<commit_message>
Modelo de Apresentação adicionado a pasta
</commit_message>
<xml_diff>
--- a/Gabriela/Documentação/Grupo 8 - ProductBacklog.xlsx
+++ b/Gabriela/Documentação/Grupo 8 - ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabes\Downloads\SIS 2°Semestre\PI - Fernando\SPRINT 1\Chech-In---Grupo8\Gabriela\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33616CF-F580-4B03-8E40-55918DE6AE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436AD6FE-9158-4749-AF7B-C4F338C0DDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,6 +119,565 @@
         <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Footer; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é uma seção importante para que o usuário ao navegar pelo site tenha maior praticidade de encontrar informações e ser direcionario para outras seções do site.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção introdutória; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é uma seção que apresenta inicialmente sobre nossos serviços de forma rápida e objetiva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção com tópicos gerais; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito importante para que o usuário que tenha acesso ao site, tenha uma visão geral sobre o que nossa equipe acredita para ter desenvolvido o projeto.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Essencial </t>
+  </si>
+  <si>
+    <t>PROT002</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção explicativa;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito que explica sobre nosso projeto, mostrando detalhes e motivação pelo qual o projeto foi criado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção de valores;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para que o cliente possa ter mais detalhes e passar maior credibilidade;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção com apresentação da equipe;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para o cliente possa conhecer e ter confiança que a equipe está preparada.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção de feedback; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito importante para que os novos clientes e/ou usuários possam ter acesso ao feedback de empresas já são nossos clientes;</t>
+    </r>
+  </si>
+  <si>
+    <t>PROT003</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção de serviços;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para que caso os clientes tenha interesse sobre nossos serviços previamente possam ir até essa seção para conhecer e entrar em contato.</t>
+    </r>
+  </si>
+  <si>
+    <t>PROT004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção de contato;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso aos nossos serviços e possa entrar em contato; </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção de login;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso ao nosso principal serviço, sendo ele as dashboards.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Seção de beneficios do negócio;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito que apresenta ao usuário como nossos serviços funcionam e no que a equipe acredita.</t>
+    </r>
+  </si>
+  <si>
+    <t>PROT005</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção para ADM; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito importante pois é através desta seção que o usuário administrador pode fazer a criação de outros usuário analista.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção de dashboard para Analista; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito para que o analista responsavel da empresa possa ter acesso aos dados para tomada de decisão;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção de suporte; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito importante para que o usuário possa ter acesso a resolução de falhas e problemas nas dashboards.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Seção de cadastro; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito para que o ADM possa ser cadastrado.</t>
+    </r>
+  </si>
+  <si>
+    <t>EC001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Pesquisa de campo;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito importante para que a equipe possa identificar problemas, falhas e bugs nos sistemas operacionais dos totens de autoatendimento.</t>
+    </r>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>DER001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Tabela usuário; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito importante para que nosso banco de dados tenha as informações necessários sos usuários que que são cadastradas na nossa plataforma.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Tabela perfil; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>é um requisito para que o sistema possa identificar o nível de permição de usuário.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Tabela cadastro-empresa;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito para ter a separação de cada empresa e atribuir que usuários pertencem a ela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Tabela de leitura;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito para que seja feita o armazenamento dos dados e os mesmos sejam transformados em interface gráfica.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve">Tabela de unidade; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito para o controle de que unidade local determinado totem pertenci.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>Tabela de Totem;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t xml:space="preserve"> é um requisito para identificação de cada máquina e que localiza-la.</t>
+    </r>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Cancelado</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Paleta de Cores</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>Congelada</t>
+  </si>
+  <si>
+    <t>Joaquim</t>
+  </si>
+  <si>
+    <t>Joaquina</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Josefina</t>
+  </si>
+  <si>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t>Team 2</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artefatos  </t>
+  </si>
+  <si>
+    <t>sigla</t>
+  </si>
+  <si>
+    <t>BPMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROTOTIPO DE TELA </t>
+  </si>
+  <si>
+    <t>PROT</t>
+  </si>
+  <si>
+    <t>USER STORIES</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>LEAN UX CANVAS</t>
+  </si>
+  <si>
+    <t>LUX</t>
+  </si>
+  <si>
+    <t>STORIE BOARD</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>MAPA DE EMPATIA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>DESENHO DE ARQUITETURA</t>
+  </si>
+  <si>
+    <t>ARQ</t>
+  </si>
+  <si>
+    <t>JORNADA DO USUÁRIO</t>
+  </si>
+  <si>
+    <t>JU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DER </t>
+  </si>
+  <si>
+    <t>DER</t>
+  </si>
+  <si>
+    <t>USE CASE</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>ENTREVISTA DE CAMPO</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Product BackLog Qualified (PBQ) - Grupo 8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
       </rPr>
       <t xml:space="preserve">Menu de páginas; </t>
@@ -129,567 +688,8 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>é um requisito para que o cliente e/ou usuário possa navegar da página principal e pelas outras paginas do site por completo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Footer; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é uma seção importante para que o usuário ao navegar pelo site tenha maior praticidade de encontrar informações e ser direcionario para outras seções do site.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção introdutória; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é uma seção que apresenta inicialmente sobre nossos serviços de forma rápida e objetiva.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção com tópicos gerais; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que o usuário que tenha acesso ao site, tenha uma visão geral sobre o que nossa equipe acredita para ter desenvolvido o projeto.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Essencial </t>
-  </si>
-  <si>
-    <t>PROT002</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção explicativa;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito que explica sobre nosso projeto, mostrando detalhes e motivação pelo qual o projeto foi criado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de valores;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente possa ter mais detalhes e passar maior credibilidade;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção com apresentação da equipe;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para o cliente possa conhecer e ter confiança que a equipe está preparada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de feedback; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que os novos clientes e/ou usuários possam ter acesso ao feedback de empresas já são nossos clientes;</t>
-    </r>
-  </si>
-  <si>
-    <t>PROT003</t>
-  </si>
-  <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de serviços;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que caso os clientes tenha interesse sobre nossos serviços previamente possam ir até essa seção para conhecer e entrar em contato.</t>
-    </r>
-  </si>
-  <si>
-    <t>PROT004</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de contato;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso aos nossos serviços e possa entrar em contato; </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de login;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso ao nosso principal serviço, sendo ele as dashboards.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de beneficios do negócio;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito que apresenta ao usuário como nossos serviços funcionam e no que a equipe acredita.</t>
-    </r>
-  </si>
-  <si>
-    <t>PROT005</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção para ADM; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante pois é através desta seção que o usuário administrador pode fazer a criação de outros usuário analista.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de dashboard para Analista; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o analista responsavel da empresa possa ter acesso aos dados para tomada de decisão;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de suporte; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que o usuário possa ter acesso a resolução de falhas e problemas nas dashboards.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de cadastro; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o ADM possa ser cadastrado.</t>
-    </r>
-  </si>
-  <si>
-    <t>EC001</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Pesquisa de campo;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que a equipe possa identificar problemas, falhas e bugs nos sistemas operacionais dos totens de autoatendimento.</t>
-    </r>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
-    <t>DER001</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela usuário; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que nosso banco de dados tenha as informações necessários sos usuários que que são cadastradas na nossa plataforma.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela perfil; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o sistema possa identificar o nível de permição de usuário.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela cadastro-empresa;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para ter a separação de cada empresa e atribuir que usuários pertencem a ela.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela de leitura;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para que seja feita o armazenamento dos dados e os mesmos sejam transformados em interface gráfica.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela de unidade; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para o controle de que unidade local determinado totem pertenci.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela de Totem;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para identificação de cada máquina e que localiza-la.</t>
-    </r>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Cancelado</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Paleta de Cores</t>
-  </si>
-  <si>
-    <t>Joana</t>
-  </si>
-  <si>
-    <t>Congelada</t>
-  </si>
-  <si>
-    <t>Joaquim</t>
-  </si>
-  <si>
-    <t>Joaquina</t>
-  </si>
-  <si>
-    <t>José</t>
-  </si>
-  <si>
-    <t>Josefina</t>
-  </si>
-  <si>
-    <t>Team 1</t>
-  </si>
-  <si>
-    <t>Team 2</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artefatos  </t>
-  </si>
-  <si>
-    <t>sigla</t>
-  </si>
-  <si>
-    <t>BPMN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROTOTIPO DE TELA </t>
-  </si>
-  <si>
-    <t>PROT</t>
-  </si>
-  <si>
-    <t>USER STORIES</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>LEAN UX CANVAS</t>
-  </si>
-  <si>
-    <t>LUX</t>
-  </si>
-  <si>
-    <t>STORIE BOARD</t>
-  </si>
-  <si>
-    <t>SB</t>
-  </si>
-  <si>
-    <t>MAPA DE EMPATIA</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>DESENHO DE ARQUITETURA</t>
-  </si>
-  <si>
-    <t>ARQ</t>
-  </si>
-  <si>
-    <t>JORNADA DO USUÁRIO</t>
-  </si>
-  <si>
-    <t>JU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DER </t>
-  </si>
-  <si>
-    <t>DER</t>
-  </si>
-  <si>
-    <t>USE CASE</t>
-  </si>
-  <si>
-    <t>UC</t>
-  </si>
-  <si>
-    <t>ENTREVISTA DE CAMPO</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>Product BackLog Qualified (PBQ) - Grupo 8</t>
+      <t>é um requisito para que o cliente e/ou usuário possa navegar pelas página principal e pelas outras paginas do site por completo.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2261,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2282,7 +2282,7 @@
     <row r="1" spans="2:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -2359,7 +2359,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>9</v>
@@ -2377,7 +2377,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="38" t="s">
         <v>9</v>
@@ -2395,7 +2395,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="38" t="s">
         <v>9</v>
@@ -2413,10 +2413,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="38" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>19</v>
       </c>
       <c r="G10" s="31"/>
     </row>
@@ -2425,13 +2425,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>9</v>
@@ -2443,13 +2443,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="38" t="s">
         <v>9</v>
@@ -2461,13 +2461,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="38" t="s">
         <v>9</v>
@@ -2479,13 +2479,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="38" t="s">
         <v>9</v>
@@ -2497,16 +2497,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="E15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="55" t="s">
-        <v>27</v>
-      </c>
       <c r="F15" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="31"/>
     </row>
@@ -2515,16 +2515,16 @@
         <v>10</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="31"/>
     </row>
@@ -2533,16 +2533,16 @@
         <v>11</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="31"/>
     </row>
@@ -2557,7 +2557,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="38" t="s">
         <v>9</v>
@@ -2569,16 +2569,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>33</v>
-      </c>
       <c r="F19" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="31"/>
     </row>
@@ -2587,16 +2587,16 @@
         <v>14</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="31"/>
     </row>
@@ -2605,16 +2605,16 @@
         <v>15</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="31"/>
     </row>
@@ -2623,16 +2623,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G22" s="31"/>
     </row>
@@ -2641,16 +2641,16 @@
         <v>17</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="38" t="s">
         <v>38</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>39</v>
       </c>
       <c r="G23" s="31"/>
     </row>
@@ -2659,16 +2659,16 @@
         <v>18</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24" s="31"/>
     </row>
@@ -2677,16 +2677,16 @@
         <v>19</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G25" s="31"/>
     </row>
@@ -2695,16 +2695,16 @@
         <v>20</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="31"/>
     </row>
@@ -2713,16 +2713,16 @@
         <v>21</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27" s="31"/>
     </row>
@@ -2731,16 +2731,16 @@
         <v>22</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G28" s="31"/>
     </row>
@@ -2749,16 +2749,16 @@
         <v>23</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G29" s="31"/>
     </row>
@@ -3119,10 +3119,10 @@
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>48</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -3131,16 +3131,16 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="64" t="s">
         <v>50</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>51</v>
       </c>
       <c r="I2" s="64"/>
       <c r="J2" s="64"/>
@@ -3151,7 +3151,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -3163,13 +3163,13 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>54</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
@@ -3178,10 +3178,10 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="63"/>
       <c r="I5" s="63"/>
@@ -3193,7 +3193,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="13"/>
     </row>
@@ -3201,28 +3201,28 @@
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3247,98 +3247,98 @@
     </row>
     <row r="16" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3363,15 +3363,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007ACFDD1B2CAD7546B60E55C07A86393C" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="181a36d502e7a0b748a7cd3f44c84256">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="93df9749-2e2e-4b03-97b6-02f28a4f49b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d2526e4fdcc8fa6c9a35e442f2e6a0" ns2:_="">
     <xsd:import namespace="93df9749-2e2e-4b03-97b6-02f28a4f49b8"/>
@@ -3503,6 +3494,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
   <ds:schemaRefs>
@@ -3513,14 +3513,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10A50834-C7D8-4E98-BE58-A043B5E9C339}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3536,4 +3528,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>